<commit_message>
Change a little bit story
This change ensures that skipping no longer triggers a waiting period.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Excel/Story/Prologue.xlsx
+++ b/Assets/StreamingAssets/Excel/Story/Prologue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Downloads\UNR\CS 425\CS425-426\Assets\StreamingAssets\Excel\Story\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92776B3-9AFC-4D1D-B607-B9F1F1D1358E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394B637D-EEFB-4277-918E-460BDC573533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added some weapon and card values
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Excel/Story/Prologue.xlsx
+++ b/Assets/StreamingAssets/Excel/Story/Prologue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Downloads\UNR\CS 425\CS425-426\Assets\StreamingAssets\Excel\Story\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNR Classes\CS 425\Unity Game\CS425-426\Assets\StreamingAssets\Excel\Story\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394B637D-EEFB-4277-918E-460BDC573533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA334B3-FEBE-4537-AF2B-470D898AE713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
     <t>Humanity depends on it.</t>
   </si>
   <si>
-    <t>Wait(1f,LoadSceneByEnum("TempMap"));</t>
+    <t>Wait(1f,LoadSceneByEnum("GameStartScene"));</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>